<commit_message>
minor bug fixes before final user studies.
</commit_message>
<xml_diff>
--- a/RoboGUI/data/ValidTrials/HRI_sim_log_2_ANALYSIS.xlsx
+++ b/RoboGUI/data/ValidTrials/HRI_sim_log_2_ANALYSIS.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="HRI_sim_log_2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>BROKE TIME</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>Avg nglect Time</t>
+  </si>
+  <si>
+    <t>Avg Cells to Go</t>
+  </si>
+  <si>
+    <t>Avg Mana</t>
+  </si>
+  <si>
+    <t>Fixes</t>
   </si>
 </sst>
 </file>
@@ -722,7 +731,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>HRI_sim_log_2!$B$5:$E$5</c:f>
+              <c:f>HRI_sim_log_2!$B$3:$E$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -743,7 +752,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>HRI_sim_log_2!$B$6:$E$6</c:f>
+              <c:f>HRI_sim_log_2!$B$4:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -772,11 +781,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="313870144"/>
-        <c:axId val="313872496"/>
+        <c:axId val="237900504"/>
+        <c:axId val="237900896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="313870144"/>
+        <c:axId val="237900504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -833,12 +842,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313872496"/>
+        <c:crossAx val="237900896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="313872496"/>
+        <c:axId val="237900896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -895,7 +904,661 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313870144"/>
+        <c:crossAx val="237900504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t># Fixes vs. Autonomy</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>HRI_sim_log_2!$B$3:$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>HRI_sim_log_2!$B$7:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="231466056"/>
+        <c:axId val="153792144"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="231466056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="153792144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="153792144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="231466056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Distance-to-go vs Autonomy</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>HRI_sim_log_2!$B$3:$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>HRI_sim_log_2!$B$5:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5.5294117647058822</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.526315789473685</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.424242424242424</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="198148152"/>
+        <c:axId val="198147760"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="198148152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="198147760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="198147760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="198148152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -984,6 +1647,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1500,20 +2243,1052 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1527,6 +3302,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1801,7 +3636,7 @@
   <dimension ref="A2:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:E6"/>
+      <selection activeCell="B5" activeCellId="1" sqref="B3:E3 B5:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1810,6 +3645,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
       <c r="K2" t="s">
         <v>14</v>
       </c>
@@ -1824,6 +3674,24 @@
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>0.2</v>
+      </c>
+      <c r="C3">
+        <v>0.4</v>
+      </c>
+      <c r="D3">
+        <v>0.9</v>
+      </c>
+      <c r="E3">
+        <v>0.95</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
       <c r="K3" t="s">
         <v>7</v>
       </c>
@@ -1839,6 +3707,9 @@
       <c r="O3" t="s">
         <v>12</v>
       </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
       <c r="Q3" t="s">
         <v>7</v>
       </c>
@@ -1857,19 +3728,27 @@
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <f>AG23</f>
+        <v>323.94117647058823</v>
       </c>
       <c r="C4">
+        <f>U42</f>
+        <v>125.05263157894737</v>
+      </c>
+      <c r="D4">
+        <f>AA38</f>
+        <v>60.606060606060609</v>
+      </c>
+      <c r="E4">
+        <f>O28</f>
+        <v>55.416666666666664</v>
+      </c>
+      <c r="J4">
+        <f>J3+1</f>
         <v>1</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
       </c>
       <c r="K4">
         <v>130</v>
@@ -1887,6 +3766,10 @@
         <f>L4-K4</f>
         <v>90</v>
       </c>
+      <c r="P4">
+        <f>P3+1</f>
+        <v>1</v>
+      </c>
       <c r="Q4">
         <v>20</v>
       </c>
@@ -1903,6 +3786,9 @@
         <f>R4-Q4</f>
         <v>332</v>
       </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
       <c r="W4" t="s">
         <v>7</v>
       </c>
@@ -1924,19 +3810,27 @@
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B5">
-        <v>0.2</v>
+        <f>AE23</f>
+        <v>5.5294117647058822</v>
       </c>
       <c r="C5">
-        <v>0.4</v>
+        <f>S42</f>
+        <v>11.526315789473685</v>
       </c>
       <c r="D5">
-        <v>0.9</v>
+        <f>Y38</f>
+        <v>10.424242424242424</v>
       </c>
       <c r="E5">
-        <v>0.95</v>
+        <f>M28</f>
+        <v>6.875</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:J27" si="0">J4+1</f>
+        <v>2</v>
       </c>
       <c r="K5">
         <v>300</v>
@@ -1951,8 +3845,12 @@
         <v>99.799700000000001</v>
       </c>
       <c r="O5">
-        <f t="shared" ref="O5:O27" si="0">L5-K5</f>
+        <f t="shared" ref="O5:O27" si="1">L5-K5</f>
         <v>29</v>
+      </c>
+      <c r="P5">
+        <f t="shared" ref="P5:P41" si="2">P4+1</f>
+        <v>2</v>
       </c>
       <c r="Q5">
         <v>370</v>
@@ -1967,8 +3865,12 @@
         <v>91.199370000000002</v>
       </c>
       <c r="U5">
-        <f t="shared" ref="U5:U41" si="1">R5-Q5</f>
+        <f t="shared" ref="U5:U41" si="3">R5-Q5</f>
         <v>78</v>
+      </c>
+      <c r="V5">
+        <f>V4+1</f>
+        <v>1</v>
       </c>
       <c r="W5">
         <v>10</v>
@@ -1986,6 +3888,9 @@
         <f>X5-W5</f>
         <v>124</v>
       </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
       <c r="AC5" t="s">
         <v>7</v>
       </c>
@@ -2004,23 +3909,27 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B6">
-        <f>AG23</f>
-        <v>323.94117647058823</v>
+        <f>AF23</f>
+        <v>50.587259352941182</v>
       </c>
       <c r="C6">
-        <f>U42</f>
-        <v>125.05263157894737</v>
+        <f>T42</f>
+        <v>36.172948973684214</v>
       </c>
       <c r="D6">
-        <f>AA38</f>
-        <v>60.606060606060609</v>
+        <f>Z38</f>
+        <v>41.732605363636374</v>
       </c>
       <c r="E6">
-        <f>O28</f>
-        <v>55.416666666666664</v>
+        <f>N28</f>
+        <v>33.407680666666671</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="K6">
         <v>770</v>
@@ -2035,8 +3944,12 @@
         <v>97.798355000000001</v>
       </c>
       <c r="O6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
       <c r="Q6">
         <v>470</v>
@@ -2051,8 +3964,12 @@
         <v>97.798659999999998</v>
       </c>
       <c r="U6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>237</v>
+      </c>
+      <c r="V6">
+        <f t="shared" ref="V6:V37" si="4">V5+1</f>
+        <v>2</v>
       </c>
       <c r="W6">
         <v>350</v>
@@ -2067,8 +3984,12 @@
         <v>88.79956</v>
       </c>
       <c r="AA6">
-        <f t="shared" ref="AA6:AA37" si="2">X6-W6</f>
+        <f t="shared" ref="AA6:AA37" si="5">X6-W6</f>
         <v>29</v>
+      </c>
+      <c r="AB6">
+        <f>AB5+1</f>
+        <v>1</v>
       </c>
       <c r="AC6">
         <v>10</v>
@@ -2088,6 +4009,29 @@
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <f>AB22</f>
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <f>P41</f>
+        <v>38</v>
+      </c>
+      <c r="D7">
+        <f>V37</f>
+        <v>33</v>
+      </c>
+      <c r="E7">
+        <f>J27</f>
+        <v>24</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
       <c r="K7">
         <v>1290</v>
       </c>
@@ -2101,8 +4045,12 @@
         <v>92.399506000000002</v>
       </c>
       <c r="O7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>81</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="Q7">
         <v>740</v>
@@ -2117,8 +4065,12 @@
         <v>94.198104999999998</v>
       </c>
       <c r="U7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>170</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="4"/>
+        <v>3</v>
       </c>
       <c r="W7">
         <v>420</v>
@@ -2133,8 +4085,12 @@
         <v>86.399289999999993</v>
       </c>
       <c r="AA7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>57</v>
+      </c>
+      <c r="AB7">
+        <f t="shared" ref="AB7:AB23" si="6">AB6+1</f>
+        <v>2</v>
       </c>
       <c r="AC7">
         <v>280</v>
@@ -2149,11 +4105,15 @@
         <v>84.199169999999995</v>
       </c>
       <c r="AG7">
-        <f t="shared" ref="AG7:AG22" si="3">AD7-AC7</f>
+        <f t="shared" ref="AG7:AG22" si="7">AD7-AC7</f>
         <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
       <c r="K8">
         <v>1720</v>
       </c>
@@ -2167,8 +4127,12 @@
         <v>51.798447000000003</v>
       </c>
       <c r="O8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="Q8">
         <v>940</v>
@@ -2183,8 +4147,12 @@
         <v>93.399640000000005</v>
       </c>
       <c r="U8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>381</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="4"/>
+        <v>4</v>
       </c>
       <c r="W8">
         <v>510</v>
@@ -2199,8 +4167,12 @@
         <v>83.999020000000002</v>
       </c>
       <c r="AA8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>65</v>
+      </c>
+      <c r="AB8">
+        <f t="shared" si="6"/>
+        <v>3</v>
       </c>
       <c r="AC8">
         <v>550</v>
@@ -2215,11 +4187,15 @@
         <v>100</v>
       </c>
       <c r="AG8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>641</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
       <c r="K9">
         <v>2290</v>
       </c>
@@ -2233,8 +4209,12 @@
         <v>15.198542</v>
       </c>
       <c r="O9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="Q9">
         <v>1350</v>
@@ -2249,8 +4229,12 @@
         <v>90.399379999999994</v>
       </c>
       <c r="U9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>65</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="4"/>
+        <v>5</v>
       </c>
       <c r="W9">
         <v>650</v>
@@ -2265,8 +4249,12 @@
         <v>92.198589999999996</v>
       </c>
       <c r="AA9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>82</v>
+      </c>
+      <c r="AB9">
+        <f t="shared" si="6"/>
+        <v>4</v>
       </c>
       <c r="AC9">
         <v>1200</v>
@@ -2281,7 +4269,7 @@
         <v>93.199799999999996</v>
       </c>
       <c r="AG9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>64</v>
       </c>
     </row>
@@ -2304,6 +4292,10 @@
       <c r="F10" t="s">
         <v>4</v>
       </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
       <c r="K10">
         <v>2450</v>
       </c>
@@ -2317,8 +4309,12 @@
         <v>19.398658999999999</v>
       </c>
       <c r="O10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>71</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
       <c r="Q10">
         <v>1430</v>
@@ -2333,8 +4329,12 @@
         <v>73.199190000000002</v>
       </c>
       <c r="U10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>56</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="4"/>
+        <v>6</v>
       </c>
       <c r="W10">
         <v>810</v>
@@ -2349,8 +4349,12 @@
         <v>92.798280000000005</v>
       </c>
       <c r="AA10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>36</v>
+      </c>
+      <c r="AB10">
+        <f t="shared" si="6"/>
+        <v>5</v>
       </c>
       <c r="AC10">
         <v>1280</v>
@@ -2365,7 +4369,7 @@
         <v>84.399320000000003</v>
       </c>
       <c r="AG10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>157</v>
       </c>
     </row>
@@ -2389,6 +4393,10 @@
       <c r="F11">
         <v>100</v>
       </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
       <c r="K11">
         <v>2770</v>
       </c>
@@ -2402,8 +4410,12 @@
         <v>20.998846</v>
       </c>
       <c r="O11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="Q11">
         <v>1510</v>
@@ -2418,8 +4430,12 @@
         <v>58.998947000000001</v>
       </c>
       <c r="U11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>64</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="4"/>
+        <v>7</v>
       </c>
       <c r="W11">
         <v>940</v>
@@ -2434,8 +4450,12 @@
         <v>94.99794</v>
       </c>
       <c r="AA11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>30</v>
+      </c>
+      <c r="AB11">
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
       <c r="AC11">
         <v>1450</v>
@@ -2450,7 +4470,7 @@
         <v>66.599140000000006</v>
       </c>
       <c r="AG11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>55</v>
       </c>
     </row>
@@ -2465,7 +4485,7 @@
         <v>220</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12:D75" si="4">C12-B12</f>
+        <f t="shared" ref="D12:D75" si="8">C12-B12</f>
         <v>90</v>
       </c>
       <c r="E12">
@@ -2474,6 +4494,10 @@
       <c r="F12">
         <v>100</v>
       </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
       <c r="K12">
         <v>2840</v>
       </c>
@@ -2487,8 +4511,12 @@
         <v>22.198889000000001</v>
       </c>
       <c r="O12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="Q12">
         <v>1610</v>
@@ -2503,8 +4531,12 @@
         <v>61.398605000000003</v>
       </c>
       <c r="U12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>88</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="W12">
         <v>1010</v>
@@ -2519,8 +4551,12 @@
         <v>100</v>
       </c>
       <c r="AA12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>45</v>
+      </c>
+      <c r="AB12">
+        <f t="shared" si="6"/>
+        <v>7</v>
       </c>
       <c r="AC12">
         <v>1510</v>
@@ -2535,7 +4571,7 @@
         <v>64.199020000000004</v>
       </c>
       <c r="AG12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>37</v>
       </c>
     </row>
@@ -2550,7 +4586,7 @@
         <v>272</v>
       </c>
       <c r="D13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>262</v>
       </c>
       <c r="E13">
@@ -2559,6 +4595,10 @@
       <c r="F13">
         <v>99.399860000000004</v>
       </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="K13">
         <v>2930</v>
       </c>
@@ -2572,8 +4612,12 @@
         <v>11.998963</v>
       </c>
       <c r="O13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>49</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="Q13">
         <v>1720</v>
@@ -2588,8 +4632,12 @@
         <v>49.198334000000003</v>
       </c>
       <c r="U13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>77</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="4"/>
+        <v>9</v>
       </c>
       <c r="W13">
         <v>1190</v>
@@ -2604,8 +4652,12 @@
         <v>95.799909999999997</v>
       </c>
       <c r="AA13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>33</v>
+      </c>
+      <c r="AB13">
+        <f t="shared" si="6"/>
+        <v>8</v>
       </c>
       <c r="AC13">
         <v>1560</v>
@@ -2620,7 +4672,7 @@
         <v>55.59854</v>
       </c>
       <c r="AG13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>162</v>
       </c>
     </row>
@@ -2635,7 +4687,7 @@
         <v>329</v>
       </c>
       <c r="D14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>29</v>
       </c>
       <c r="E14">
@@ -2644,6 +4696,10 @@
       <c r="F14">
         <v>99.799700000000001</v>
       </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
       <c r="K14">
         <v>3280</v>
       </c>
@@ -2657,8 +4713,12 @@
         <v>23.199107999999999</v>
       </c>
       <c r="O14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="Q14">
         <v>1820</v>
@@ -2673,8 +4733,12 @@
         <v>28.598262999999999</v>
       </c>
       <c r="U14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>30</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="4"/>
+        <v>10</v>
       </c>
       <c r="W14">
         <v>1420</v>
@@ -2689,8 +4753,12 @@
         <v>78.399259999999998</v>
       </c>
       <c r="AA14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>40</v>
+      </c>
+      <c r="AB14">
+        <f t="shared" si="6"/>
+        <v>9</v>
       </c>
       <c r="AC14">
         <v>1750</v>
@@ -2705,7 +4773,7 @@
         <v>41.398299999999999</v>
       </c>
       <c r="AG14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>59</v>
       </c>
     </row>
@@ -2720,7 +4788,7 @@
         <v>352</v>
       </c>
       <c r="D15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>332</v>
       </c>
       <c r="E15">
@@ -2729,6 +4797,10 @@
       <c r="F15">
         <v>93.799639999999997</v>
       </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
       <c r="K15">
         <v>3430</v>
       </c>
@@ -2742,8 +4814,12 @@
         <v>10.799184</v>
       </c>
       <c r="O15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="2"/>
+        <v>12</v>
       </c>
       <c r="Q15">
         <v>1870</v>
@@ -2758,8 +4834,12 @@
         <v>21.398426000000001</v>
       </c>
       <c r="U15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>217</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="4"/>
+        <v>11</v>
       </c>
       <c r="W15">
         <v>1560</v>
@@ -2774,8 +4854,12 @@
         <v>56.798830000000002</v>
       </c>
       <c r="AA15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>57</v>
+      </c>
+      <c r="AB15">
+        <f t="shared" si="6"/>
+        <v>10</v>
       </c>
       <c r="AC15">
         <v>1810</v>
@@ -2790,7 +4874,7 @@
         <v>35.398249999999997</v>
       </c>
       <c r="AG15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>22</v>
       </c>
     </row>
@@ -2805,7 +4889,7 @@
         <v>379</v>
       </c>
       <c r="D16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>29</v>
       </c>
       <c r="E16">
@@ -2814,6 +4898,10 @@
       <c r="F16">
         <v>88.79956</v>
       </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
       <c r="K16">
         <v>3580</v>
       </c>
@@ -2827,8 +4915,12 @@
         <v>18.199255000000001</v>
       </c>
       <c r="O16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="2"/>
+        <v>13</v>
       </c>
       <c r="Q16">
         <v>2110</v>
@@ -2843,8 +4935,12 @@
         <v>25.598644</v>
       </c>
       <c r="U16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>390</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="4"/>
+        <v>12</v>
       </c>
       <c r="W16">
         <v>1810</v>
@@ -2859,8 +4955,12 @@
         <v>22.998280000000001</v>
       </c>
       <c r="AA16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>64</v>
+      </c>
+      <c r="AB16">
+        <f t="shared" si="6"/>
+        <v>11</v>
       </c>
       <c r="AC16">
         <v>1850</v>
@@ -2875,7 +4975,7 @@
         <v>23.998322000000002</v>
       </c>
       <c r="AG16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>85</v>
       </c>
     </row>
@@ -2890,7 +4990,7 @@
         <v>448</v>
       </c>
       <c r="D17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>78</v>
       </c>
       <c r="E17">
@@ -2899,6 +4999,10 @@
       <c r="F17">
         <v>91.199370000000002</v>
       </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
       <c r="K17">
         <v>3710</v>
       </c>
@@ -2912,8 +5016,12 @@
         <v>15.399359</v>
       </c>
       <c r="O17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>66</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="2"/>
+        <v>14</v>
       </c>
       <c r="Q17">
         <v>2530</v>
@@ -2928,8 +5036,12 @@
         <v>24.598745000000001</v>
       </c>
       <c r="U17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>131</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="4"/>
+        <v>13</v>
       </c>
       <c r="W17">
         <v>2120</v>
@@ -2944,8 +5056,12 @@
         <v>14.398463</v>
       </c>
       <c r="AA17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>40</v>
+      </c>
+      <c r="AB17">
+        <f t="shared" si="6"/>
+        <v>12</v>
       </c>
       <c r="AC17">
         <v>1940</v>
@@ -2960,7 +5076,7 @@
         <v>24.398361000000001</v>
       </c>
       <c r="AG17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>53</v>
       </c>
     </row>
@@ -2975,7 +5091,7 @@
         <v>477</v>
       </c>
       <c r="D18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>57</v>
       </c>
       <c r="E18">
@@ -2984,6 +5100,10 @@
       <c r="F18">
         <v>86.399289999999993</v>
       </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
       <c r="K18">
         <v>3850</v>
       </c>
@@ -2997,8 +5117,12 @@
         <v>15.59942</v>
       </c>
       <c r="O18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="2"/>
+        <v>15</v>
       </c>
       <c r="Q18">
         <v>2690</v>
@@ -3013,8 +5137,12 @@
         <v>29.198801</v>
       </c>
       <c r="U18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>52</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="4"/>
+        <v>14</v>
       </c>
       <c r="W18">
         <v>2220</v>
@@ -3029,8 +5157,12 @@
         <v>13.798518</v>
       </c>
       <c r="AA18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>47</v>
+      </c>
+      <c r="AB18">
+        <f t="shared" si="6"/>
+        <v>13</v>
       </c>
       <c r="AC18">
         <v>2010</v>
@@ -3045,7 +5177,7 @@
         <v>24.198398999999998</v>
       </c>
       <c r="AG18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>37</v>
       </c>
     </row>
@@ -3060,7 +5192,7 @@
         <v>521</v>
       </c>
       <c r="D19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>241</v>
       </c>
       <c r="E19">
@@ -3069,6 +5201,10 @@
       <c r="F19">
         <v>84.199169999999995</v>
       </c>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
       <c r="K19">
         <v>4020</v>
       </c>
@@ -3082,8 +5218,12 @@
         <v>15.199460999999999</v>
       </c>
       <c r="O19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="2"/>
+        <v>16</v>
       </c>
       <c r="Q19">
         <v>2780</v>
@@ -3098,8 +5238,12 @@
         <v>19.398916</v>
       </c>
       <c r="U19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>130</v>
+      </c>
+      <c r="V19">
+        <f t="shared" si="4"/>
+        <v>15</v>
       </c>
       <c r="W19">
         <v>2350</v>
@@ -3114,8 +5258,12 @@
         <v>21.798591999999999</v>
       </c>
       <c r="AA19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>73</v>
+      </c>
+      <c r="AB19">
+        <f t="shared" si="6"/>
+        <v>14</v>
       </c>
       <c r="AC19">
         <v>2050</v>
@@ -3130,7 +5278,7 @@
         <v>15.398441</v>
       </c>
       <c r="AG19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>59</v>
       </c>
     </row>
@@ -3145,7 +5293,7 @@
         <v>575</v>
       </c>
       <c r="D20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>65</v>
       </c>
       <c r="E20">
@@ -3154,6 +5302,10 @@
       <c r="F20">
         <v>83.999020000000002</v>
       </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
       <c r="K20">
         <v>4150</v>
       </c>
@@ -3167,8 +5319,12 @@
         <v>18.399536000000001</v>
       </c>
       <c r="O20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="2"/>
+        <v>17</v>
       </c>
       <c r="Q20">
         <v>2950</v>
@@ -3183,8 +5339,12 @@
         <v>11.798988</v>
       </c>
       <c r="U20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>140</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="4"/>
+        <v>16</v>
       </c>
       <c r="W20">
         <v>2480</v>
@@ -3199,8 +5359,12 @@
         <v>15.998684000000001</v>
       </c>
       <c r="AA20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>77</v>
+      </c>
+      <c r="AB20">
+        <f t="shared" si="6"/>
+        <v>15</v>
       </c>
       <c r="AC20">
         <v>2110</v>
@@ -3215,7 +5379,7 @@
         <v>17.798496</v>
       </c>
       <c r="AG20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>124</v>
       </c>
     </row>
@@ -3230,7 +5394,7 @@
         <v>707</v>
       </c>
       <c r="D21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>237</v>
       </c>
       <c r="E21">
@@ -3239,6 +5403,10 @@
       <c r="F21">
         <v>97.798659999999998</v>
       </c>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
       <c r="K21">
         <v>4590</v>
       </c>
@@ -3252,8 +5420,12 @@
         <v>34.999687000000002</v>
       </c>
       <c r="O21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="2"/>
+        <v>18</v>
       </c>
       <c r="Q21">
         <v>3110</v>
@@ -3268,8 +5440,12 @@
         <v>16.599014</v>
       </c>
       <c r="U21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>62</v>
+      </c>
+      <c r="V21">
+        <f t="shared" si="4"/>
+        <v>17</v>
       </c>
       <c r="W21">
         <v>2650</v>
@@ -3284,8 +5460,12 @@
         <v>24.198820000000001</v>
       </c>
       <c r="AA21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>120</v>
+      </c>
+      <c r="AB21">
+        <f t="shared" si="6"/>
+        <v>16</v>
       </c>
       <c r="AC21">
         <v>2250</v>
@@ -3300,7 +5480,7 @@
         <v>13.799961</v>
       </c>
       <c r="AG21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>3295</v>
       </c>
     </row>
@@ -3315,7 +5495,7 @@
         <v>732</v>
       </c>
       <c r="D22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>82</v>
       </c>
       <c r="E22">
@@ -3324,6 +5504,10 @@
       <c r="F22">
         <v>92.198589999999996</v>
       </c>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
       <c r="K22">
         <v>4710</v>
       </c>
@@ -3337,8 +5521,12 @@
         <v>18.999779</v>
       </c>
       <c r="O22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>31</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="2"/>
+        <v>19</v>
       </c>
       <c r="Q22">
         <v>3190</v>
@@ -3353,8 +5541,12 @@
         <v>18.999054000000001</v>
       </c>
       <c r="U22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>51</v>
+      </c>
+      <c r="V22">
+        <f t="shared" si="4"/>
+        <v>18</v>
       </c>
       <c r="W22">
         <v>2940</v>
@@ -3369,8 +5561,12 @@
         <v>17.798947999999999</v>
       </c>
       <c r="AA22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>16</v>
+      </c>
+      <c r="AB22">
+        <f t="shared" si="6"/>
+        <v>17</v>
       </c>
       <c r="AC22">
         <v>5570</v>
@@ -3385,7 +5581,7 @@
         <v>16.000029000000001</v>
       </c>
       <c r="AG22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>154</v>
       </c>
     </row>
@@ -3400,7 +5596,7 @@
         <v>818</v>
       </c>
       <c r="D23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>48</v>
       </c>
       <c r="E23">
@@ -3409,6 +5605,10 @@
       <c r="F23">
         <v>97.798355000000001</v>
       </c>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
       <c r="K23">
         <v>4790</v>
       </c>
@@ -3422,8 +5622,12 @@
         <v>13.999808</v>
       </c>
       <c r="O23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="2"/>
+        <v>20</v>
       </c>
       <c r="Q23">
         <v>3260</v>
@@ -3438,8 +5642,12 @@
         <v>16.999123000000001</v>
       </c>
       <c r="U23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>81</v>
+      </c>
+      <c r="V23">
+        <f t="shared" si="4"/>
+        <v>19</v>
       </c>
       <c r="W23">
         <v>3010</v>
@@ -3454,8 +5662,20 @@
         <v>13.398978</v>
       </c>
       <c r="AA23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>33</v>
+      </c>
+      <c r="AB23">
+        <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
+      <c r="AE23">
+        <f>AVERAGE(AE6:AE22)</f>
+        <v>5.5294117647058822</v>
+      </c>
+      <c r="AF23">
+        <f>AVERAGE(AF6:AF22)</f>
+        <v>50.587259352941182</v>
       </c>
       <c r="AG23">
         <f>AVERAGE(AG6:AG22)</f>
@@ -3473,7 +5693,7 @@
         <v>846</v>
       </c>
       <c r="D24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>36</v>
       </c>
       <c r="E24">
@@ -3482,6 +5702,10 @@
       <c r="F24">
         <v>92.798280000000005</v>
       </c>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
       <c r="K24">
         <v>4900</v>
       </c>
@@ -3495,8 +5719,12 @@
         <v>15.799846000000001</v>
       </c>
       <c r="O24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="2"/>
+        <v>21</v>
       </c>
       <c r="Q24">
         <v>3360</v>
@@ -3511,8 +5739,12 @@
         <v>15.799151</v>
       </c>
       <c r="U24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>30</v>
+      </c>
+      <c r="V24">
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
       <c r="W24">
         <v>3360</v>
@@ -3527,7 +5759,7 @@
         <v>14.999176</v>
       </c>
       <c r="AA24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>81</v>
       </c>
     </row>
@@ -3542,7 +5774,7 @@
         <v>910</v>
       </c>
       <c r="D25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>170</v>
       </c>
       <c r="E25">
@@ -3551,6 +5783,10 @@
       <c r="F25">
         <v>94.198104999999998</v>
       </c>
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
       <c r="K25">
         <v>4970</v>
       </c>
@@ -3564,8 +5800,12 @@
         <v>31.599981</v>
       </c>
       <c r="O25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>285</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="2"/>
+        <v>22</v>
       </c>
       <c r="Q25">
         <v>3440</v>
@@ -3580,8 +5820,12 @@
         <v>22.599233999999999</v>
       </c>
       <c r="U25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>154</v>
+      </c>
+      <c r="V25">
+        <f t="shared" si="4"/>
+        <v>21</v>
       </c>
       <c r="W25">
         <v>3540</v>
@@ -3596,7 +5840,7 @@
         <v>22.399346999999999</v>
       </c>
       <c r="AA25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>219</v>
       </c>
     </row>
@@ -3611,7 +5855,7 @@
         <v>970</v>
       </c>
       <c r="D26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>30</v>
       </c>
       <c r="E26">
@@ -3620,6 +5864,10 @@
       <c r="F26">
         <v>94.99794</v>
       </c>
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
       <c r="K26">
         <v>5470</v>
       </c>
@@ -3633,8 +5881,12 @@
         <v>26.799934</v>
       </c>
       <c r="O26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="2"/>
+        <v>23</v>
       </c>
       <c r="Q26">
         <v>3610</v>
@@ -3649,8 +5901,12 @@
         <v>28.799334000000002</v>
       </c>
       <c r="U26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>129</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="4"/>
+        <v>22</v>
       </c>
       <c r="W26">
         <v>3920</v>
@@ -3665,7 +5921,7 @@
         <v>11.399438999999999</v>
       </c>
       <c r="AA26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>56</v>
       </c>
     </row>
@@ -3680,7 +5936,7 @@
         <v>1055</v>
       </c>
       <c r="D27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>45</v>
       </c>
       <c r="E27">
@@ -3689,6 +5945,10 @@
       <c r="F27">
         <v>100</v>
       </c>
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
       <c r="K27">
         <v>5790</v>
       </c>
@@ -3702,8 +5962,12 @@
         <v>11.200070999999999</v>
       </c>
       <c r="O27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>74</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="2"/>
+        <v>24</v>
       </c>
       <c r="Q27">
         <v>3760</v>
@@ -3718,8 +5982,12 @@
         <v>17.399391000000001</v>
       </c>
       <c r="U27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>83</v>
+      </c>
+      <c r="V27">
+        <f t="shared" si="4"/>
+        <v>23</v>
       </c>
       <c r="W27">
         <v>4120</v>
@@ -3734,7 +6002,7 @@
         <v>20.599506000000002</v>
       </c>
       <c r="AA27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
     </row>
@@ -3749,7 +6017,7 @@
         <v>1191</v>
       </c>
       <c r="D28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>641</v>
       </c>
       <c r="E28">
@@ -3757,11 +6025,23 @@
       </c>
       <c r="F28">
         <v>100</v>
+      </c>
+      <c r="M28">
+        <f>AVERAGE(M4:M27)</f>
+        <v>6.875</v>
+      </c>
+      <c r="N28">
+        <f>AVERAGE(N4:N27)</f>
+        <v>33.407680666666671</v>
       </c>
       <c r="O28">
         <f>AVERAGE(O4:O27)</f>
         <v>55.416666666666664</v>
       </c>
+      <c r="P28">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
       <c r="Q28">
         <v>3870</v>
       </c>
@@ -3775,8 +6055,12 @@
         <v>11.799431999999999</v>
       </c>
       <c r="U28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>53</v>
+      </c>
+      <c r="V28">
+        <f t="shared" si="4"/>
+        <v>24</v>
       </c>
       <c r="W28">
         <v>4230</v>
@@ -3791,7 +6075,7 @@
         <v>12.799631</v>
       </c>
       <c r="AA28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>143</v>
       </c>
     </row>
@@ -3806,7 +6090,7 @@
         <v>1223</v>
       </c>
       <c r="D29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>33</v>
       </c>
       <c r="E29">
@@ -3815,6 +6099,10 @@
       <c r="F29">
         <v>95.799909999999997</v>
       </c>
+      <c r="P29">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
       <c r="Q29">
         <v>3950</v>
       </c>
@@ -3828,8 +6116,12 @@
         <v>13.399554999999999</v>
       </c>
       <c r="U29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>259</v>
+      </c>
+      <c r="V29">
+        <f t="shared" si="4"/>
+        <v>25</v>
       </c>
       <c r="W29">
         <v>4420</v>
@@ -3844,7 +6136,7 @@
         <v>13.399647</v>
       </c>
       <c r="AA29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
     </row>
@@ -3859,7 +6151,7 @@
         <v>1264</v>
       </c>
       <c r="D30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>64</v>
       </c>
       <c r="E30">
@@ -3868,6 +6160,10 @@
       <c r="F30">
         <v>93.199799999999996</v>
       </c>
+      <c r="P30">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
       <c r="Q30">
         <v>4240</v>
       </c>
@@ -3881,8 +6177,12 @@
         <v>14.999577499999999</v>
       </c>
       <c r="U30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>34</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="4"/>
+        <v>26</v>
       </c>
       <c r="W30">
         <v>4640</v>
@@ -3897,7 +6197,7 @@
         <v>23.599720000000001</v>
       </c>
       <c r="AA30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
     </row>
@@ -3912,7 +6212,7 @@
         <v>1321</v>
       </c>
       <c r="D31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>381</v>
       </c>
       <c r="E31">
@@ -3921,6 +6221,10 @@
       <c r="F31">
         <v>93.399640000000005</v>
       </c>
+      <c r="P31">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
       <c r="Q31">
         <v>4300</v>
       </c>
@@ -3934,8 +6238,12 @@
         <v>18.199614</v>
       </c>
       <c r="U31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>47</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="4"/>
+        <v>27</v>
       </c>
       <c r="W31">
         <v>4730</v>
@@ -3950,7 +6258,7 @@
         <v>12.199790999999999</v>
       </c>
       <c r="AA31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
     </row>
@@ -3965,7 +6273,7 @@
         <v>1371</v>
       </c>
       <c r="D32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>81</v>
       </c>
       <c r="E32">
@@ -3974,6 +6282,10 @@
       <c r="F32">
         <v>92.399506000000002</v>
       </c>
+      <c r="P32">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
       <c r="Q32">
         <v>4360</v>
       </c>
@@ -3987,8 +6299,12 @@
         <v>30.399708</v>
       </c>
       <c r="U32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>277</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="4"/>
+        <v>28</v>
       </c>
       <c r="W32">
         <v>4870</v>
@@ -4003,7 +6319,7 @@
         <v>12.999863</v>
       </c>
       <c r="AA32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>115</v>
       </c>
     </row>
@@ -4018,7 +6334,7 @@
         <v>1415</v>
       </c>
       <c r="D33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>65</v>
       </c>
       <c r="E33">
@@ -4027,6 +6343,10 @@
       <c r="F33">
         <v>90.399379999999994</v>
       </c>
+      <c r="P33">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
       <c r="Q33">
         <v>4670</v>
       </c>
@@ -4040,8 +6360,12 @@
         <v>22.999756000000001</v>
       </c>
       <c r="U33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>37</v>
+      </c>
+      <c r="V33">
+        <f t="shared" si="4"/>
+        <v>29</v>
       </c>
       <c r="W33">
         <v>5010</v>
@@ -4056,7 +6380,7 @@
         <v>12.399875</v>
       </c>
       <c r="AA33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
     </row>
@@ -4071,7 +6395,7 @@
         <v>1437</v>
       </c>
       <c r="D34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>157</v>
       </c>
       <c r="E34">
@@ -4080,6 +6404,10 @@
       <c r="F34">
         <v>84.399320000000003</v>
       </c>
+      <c r="P34">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
       <c r="Q34">
         <v>4710</v>
       </c>
@@ -4093,8 +6421,12 @@
         <v>12.399820999999999</v>
       </c>
       <c r="U34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>161</v>
+      </c>
+      <c r="V34">
+        <f t="shared" si="4"/>
+        <v>30</v>
       </c>
       <c r="W34">
         <v>5280</v>
@@ -4109,7 +6441,7 @@
         <v>38.399920000000002</v>
       </c>
       <c r="AA34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>68</v>
       </c>
     </row>
@@ -4124,7 +6456,7 @@
         <v>1460</v>
       </c>
       <c r="D35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>40</v>
       </c>
       <c r="E35">
@@ -4133,6 +6465,10 @@
       <c r="F35">
         <v>78.399259999999998</v>
       </c>
+      <c r="P35">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
       <c r="Q35">
         <v>4890</v>
       </c>
@@ -4146,8 +6482,12 @@
         <v>14.799894999999999</v>
       </c>
       <c r="U35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>216</v>
+      </c>
+      <c r="V35">
+        <f t="shared" si="4"/>
+        <v>31</v>
       </c>
       <c r="W35">
         <v>5420</v>
@@ -4162,7 +6502,7 @@
         <v>30.999911999999998</v>
       </c>
       <c r="AA35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>54</v>
       </c>
     </row>
@@ -4177,7 +6517,7 @@
         <v>1486</v>
       </c>
       <c r="D36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>56</v>
       </c>
       <c r="E36">
@@ -4186,6 +6526,10 @@
       <c r="F36">
         <v>73.199190000000002</v>
       </c>
+      <c r="P36">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
       <c r="Q36">
         <v>5160</v>
       </c>
@@ -4199,8 +6543,12 @@
         <v>34.999890000000001</v>
       </c>
       <c r="U36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>225</v>
+      </c>
+      <c r="V36">
+        <f t="shared" si="4"/>
+        <v>32</v>
       </c>
       <c r="W36">
         <v>5750</v>
@@ -4215,7 +6563,7 @@
         <v>13.200063999999999</v>
       </c>
       <c r="AA36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>70</v>
       </c>
     </row>
@@ -4230,7 +6578,7 @@
         <v>1505</v>
       </c>
       <c r="D37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="E37">
@@ -4239,6 +6587,10 @@
       <c r="F37">
         <v>66.599140000000006</v>
       </c>
+      <c r="P37">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
       <c r="Q37">
         <v>5400</v>
       </c>
@@ -4252,8 +6604,12 @@
         <v>33.999885999999996</v>
       </c>
       <c r="U37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>35</v>
+      </c>
+      <c r="V37">
+        <f t="shared" si="4"/>
+        <v>33</v>
       </c>
       <c r="W37">
         <v>5960</v>
@@ -4268,7 +6624,7 @@
         <v>23.200123000000001</v>
       </c>
       <c r="AA37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>26</v>
       </c>
     </row>
@@ -4283,7 +6639,7 @@
         <v>1547</v>
       </c>
       <c r="D38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>37</v>
       </c>
       <c r="E38">
@@ -4292,6 +6648,10 @@
       <c r="F38">
         <v>64.199020000000004</v>
       </c>
+      <c r="P38">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
       <c r="Q38">
         <v>5500</v>
       </c>
@@ -4305,8 +6665,16 @@
         <v>19.599945000000002</v>
       </c>
       <c r="U38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>22</v>
+      </c>
+      <c r="Y38">
+        <f>AVERAGE(Y5:Y37)</f>
+        <v>10.424242424242424</v>
+      </c>
+      <c r="Z38">
+        <f>AVERAGE(Z5:Z37)</f>
+        <v>41.732605363636374</v>
       </c>
       <c r="AA38">
         <f>AVERAGE(AA5:AA37)</f>
@@ -4324,7 +6692,7 @@
         <v>1574</v>
       </c>
       <c r="D39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>64</v>
       </c>
       <c r="E39">
@@ -4333,6 +6701,10 @@
       <c r="F39">
         <v>58.998947000000001</v>
       </c>
+      <c r="P39">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
       <c r="Q39">
         <v>5550</v>
       </c>
@@ -4346,7 +6718,7 @@
         <v>10.199965499999999</v>
       </c>
       <c r="U39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
     </row>
@@ -4361,7 +6733,7 @@
         <v>1617</v>
       </c>
       <c r="D40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>57</v>
       </c>
       <c r="E40">
@@ -4370,6 +6742,10 @@
       <c r="F40">
         <v>56.798830000000002</v>
       </c>
+      <c r="P40">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
       <c r="Q40">
         <v>5620</v>
       </c>
@@ -4383,7 +6759,7 @@
         <v>21.800013</v>
       </c>
       <c r="U40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>81</v>
       </c>
     </row>
@@ -4398,7 +6774,7 @@
         <v>1698</v>
       </c>
       <c r="D41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>88</v>
       </c>
       <c r="E41">
@@ -4407,6 +6783,10 @@
       <c r="F41">
         <v>61.398605000000003</v>
       </c>
+      <c r="P41">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
       <c r="Q41">
         <v>5720</v>
       </c>
@@ -4420,7 +6800,7 @@
         <v>13.600047999999999</v>
       </c>
       <c r="U41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>46</v>
       </c>
     </row>
@@ -4435,7 +6815,7 @@
         <v>1722</v>
       </c>
       <c r="D42">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>162</v>
       </c>
       <c r="E42">
@@ -4443,6 +6823,14 @@
       </c>
       <c r="F42">
         <v>55.59854</v>
+      </c>
+      <c r="S42">
+        <f>AVERAGE(S4:S41)</f>
+        <v>11.526315789473685</v>
+      </c>
+      <c r="T42">
+        <f>AVERAGE(T4:T41)</f>
+        <v>36.172948973684214</v>
       </c>
       <c r="U42">
         <f>AVERAGE(U4:U41)</f>
@@ -4460,7 +6848,7 @@
         <v>1756</v>
       </c>
       <c r="D43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>36</v>
       </c>
       <c r="E43">
@@ -4481,7 +6869,7 @@
         <v>1797</v>
       </c>
       <c r="D44">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>77</v>
       </c>
       <c r="E44">
@@ -4502,7 +6890,7 @@
         <v>1809</v>
       </c>
       <c r="D45">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>59</v>
       </c>
       <c r="E45">
@@ -4523,7 +6911,7 @@
         <v>1832</v>
       </c>
       <c r="D46">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>22</v>
       </c>
       <c r="E46">
@@ -4544,7 +6932,7 @@
         <v>1850</v>
       </c>
       <c r="D47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>30</v>
       </c>
       <c r="E47">
@@ -4565,7 +6953,7 @@
         <v>1874</v>
       </c>
       <c r="D48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>64</v>
       </c>
       <c r="E48">
@@ -4586,7 +6974,7 @@
         <v>1935</v>
       </c>
       <c r="D49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>85</v>
       </c>
       <c r="E49">
@@ -4607,7 +6995,7 @@
         <v>1993</v>
       </c>
       <c r="D50">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>53</v>
       </c>
       <c r="E50">
@@ -4628,7 +7016,7 @@
         <v>2047</v>
       </c>
       <c r="D51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>37</v>
       </c>
       <c r="E51">
@@ -4649,7 +7037,7 @@
         <v>2087</v>
       </c>
       <c r="D52">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>217</v>
       </c>
       <c r="E52">
@@ -4670,7 +7058,7 @@
         <v>2109</v>
       </c>
       <c r="D53">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>59</v>
       </c>
       <c r="E53">
@@ -4691,7 +7079,7 @@
         <v>2160</v>
       </c>
       <c r="D54">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>40</v>
       </c>
       <c r="E54">
@@ -4712,7 +7100,7 @@
         <v>2234</v>
       </c>
       <c r="D55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>124</v>
       </c>
       <c r="E55">
@@ -4733,7 +7121,7 @@
         <v>2267</v>
       </c>
       <c r="D56">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>47</v>
       </c>
       <c r="E56">
@@ -4754,7 +7142,7 @@
         <v>2331</v>
       </c>
       <c r="D57">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>41</v>
       </c>
       <c r="E57">
@@ -4775,7 +7163,7 @@
         <v>2423</v>
       </c>
       <c r="D58">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>73</v>
       </c>
       <c r="E58">
@@ -4796,7 +7184,7 @@
         <v>2500</v>
       </c>
       <c r="D59">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>390</v>
       </c>
       <c r="E59">
@@ -4817,7 +7205,7 @@
         <v>2521</v>
       </c>
       <c r="D60">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>71</v>
       </c>
       <c r="E60">
@@ -4838,7 +7226,7 @@
         <v>2557</v>
       </c>
       <c r="D61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>77</v>
       </c>
       <c r="E61">
@@ -4859,7 +7247,7 @@
         <v>2661</v>
       </c>
       <c r="D62">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>131</v>
       </c>
       <c r="E62">
@@ -4880,7 +7268,7 @@
         <v>2742</v>
       </c>
       <c r="D63">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>52</v>
       </c>
       <c r="E63">
@@ -4901,7 +7289,7 @@
         <v>2770</v>
       </c>
       <c r="D64">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>120</v>
       </c>
       <c r="E64">
@@ -4922,7 +7310,7 @@
         <v>2807</v>
       </c>
       <c r="D65">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>37</v>
       </c>
       <c r="E65">
@@ -4943,7 +7331,7 @@
         <v>2869</v>
       </c>
       <c r="D66">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>29</v>
       </c>
       <c r="E66">
@@ -4964,7 +7352,7 @@
         <v>2910</v>
       </c>
       <c r="D67">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>130</v>
       </c>
       <c r="E67">
@@ -4985,7 +7373,7 @@
         <v>2956</v>
       </c>
       <c r="D68">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="E68">
@@ -5006,7 +7394,7 @@
         <v>2979</v>
       </c>
       <c r="D69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>49</v>
       </c>
       <c r="E69">
@@ -5027,7 +7415,7 @@
         <v>3043</v>
       </c>
       <c r="D70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>33</v>
       </c>
       <c r="E70">
@@ -5048,7 +7436,7 @@
         <v>3090</v>
       </c>
       <c r="D71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>140</v>
       </c>
       <c r="E71">
@@ -5069,7 +7457,7 @@
         <v>3172</v>
       </c>
       <c r="D72">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>62</v>
       </c>
       <c r="E72">
@@ -5090,7 +7478,7 @@
         <v>3241</v>
       </c>
       <c r="D73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>51</v>
       </c>
       <c r="E73">
@@ -5111,7 +7499,7 @@
         <v>3320</v>
       </c>
       <c r="D74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>40</v>
       </c>
       <c r="E74">
@@ -5132,7 +7520,7 @@
         <v>3341</v>
       </c>
       <c r="D75">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>81</v>
       </c>
       <c r="E75">
@@ -5153,7 +7541,7 @@
         <v>3390</v>
       </c>
       <c r="D76">
-        <f t="shared" ref="D76:D122" si="5">C76-B76</f>
+        <f t="shared" ref="D76:D122" si="9">C76-B76</f>
         <v>30</v>
       </c>
       <c r="E76">
@@ -5174,7 +7562,7 @@
         <v>3441</v>
       </c>
       <c r="D77">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>81</v>
       </c>
       <c r="E77">
@@ -5195,7 +7583,7 @@
         <v>3473</v>
       </c>
       <c r="D78">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>43</v>
       </c>
       <c r="E78">
@@ -5216,7 +7604,7 @@
         <v>3594</v>
       </c>
       <c r="D79">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>154</v>
       </c>
       <c r="E79">
@@ -5237,7 +7625,7 @@
         <v>3625</v>
       </c>
       <c r="D80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>45</v>
       </c>
       <c r="E80">
@@ -5258,7 +7646,7 @@
         <v>3739</v>
       </c>
       <c r="D81">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>129</v>
       </c>
       <c r="E81">
@@ -5279,7 +7667,7 @@
         <v>3759</v>
       </c>
       <c r="D82">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>219</v>
       </c>
       <c r="E82">
@@ -5300,7 +7688,7 @@
         <v>3776</v>
       </c>
       <c r="D83">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>66</v>
       </c>
       <c r="E83">
@@ -5321,7 +7709,7 @@
         <v>3843</v>
       </c>
       <c r="D84">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>83</v>
       </c>
       <c r="E84">
@@ -5342,7 +7730,7 @@
         <v>3888</v>
       </c>
       <c r="D85">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>38</v>
       </c>
       <c r="E85">
@@ -5363,7 +7751,7 @@
         <v>3923</v>
       </c>
       <c r="D86">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>53</v>
       </c>
       <c r="E86">
@@ -5384,7 +7772,7 @@
         <v>3976</v>
       </c>
       <c r="D87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>56</v>
       </c>
       <c r="E87">
@@ -5405,7 +7793,7 @@
         <v>4053</v>
       </c>
       <c r="D88">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>33</v>
       </c>
       <c r="E88">
@@ -5426,7 +7814,7 @@
         <v>4138</v>
       </c>
       <c r="D89">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>18</v>
       </c>
       <c r="E89">
@@ -5447,7 +7835,7 @@
         <v>4182</v>
       </c>
       <c r="D90">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>32</v>
       </c>
       <c r="E90">
@@ -5468,7 +7856,7 @@
         <v>4209</v>
       </c>
       <c r="D91">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>259</v>
       </c>
       <c r="E91">
@@ -5489,7 +7877,7 @@
         <v>4274</v>
       </c>
       <c r="D92">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>34</v>
       </c>
       <c r="E92">
@@ -5510,7 +7898,7 @@
         <v>4347</v>
       </c>
       <c r="D93">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>47</v>
       </c>
       <c r="E93">
@@ -5531,7 +7919,7 @@
         <v>4373</v>
       </c>
       <c r="D94">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>143</v>
       </c>
       <c r="E94">
@@ -5552,7 +7940,7 @@
         <v>4432</v>
       </c>
       <c r="D95">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="E95">
@@ -5573,7 +7961,7 @@
         <v>4607</v>
       </c>
       <c r="D96">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>17</v>
       </c>
       <c r="E96">
@@ -5594,7 +7982,7 @@
         <v>4637</v>
       </c>
       <c r="D97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>277</v>
       </c>
       <c r="E97">
@@ -5615,7 +8003,7 @@
         <v>4655</v>
       </c>
       <c r="D98">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
       <c r="E98">
@@ -5636,7 +8024,7 @@
         <v>4707</v>
       </c>
       <c r="D99">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>37</v>
       </c>
       <c r="E99">
@@ -5657,7 +8045,7 @@
         <v>4741</v>
       </c>
       <c r="D100">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>31</v>
       </c>
       <c r="E100">
@@ -5678,7 +8066,7 @@
         <v>4758</v>
       </c>
       <c r="D101">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>28</v>
       </c>
       <c r="E101">
@@ -5699,7 +8087,7 @@
         <v>4824</v>
       </c>
       <c r="D102">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>34</v>
       </c>
       <c r="E102">
@@ -5720,7 +8108,7 @@
         <v>4871</v>
       </c>
       <c r="D103">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>161</v>
       </c>
       <c r="E103">
@@ -5741,7 +8129,7 @@
         <v>4945</v>
       </c>
       <c r="D104">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>45</v>
       </c>
       <c r="E104">
@@ -5762,7 +8150,7 @@
         <v>4985</v>
       </c>
       <c r="D105">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>115</v>
       </c>
       <c r="E105">
@@ -5783,7 +8171,7 @@
         <v>5037</v>
       </c>
       <c r="D106">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>27</v>
       </c>
       <c r="E106">
@@ -5804,7 +8192,7 @@
         <v>5106</v>
       </c>
       <c r="D107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>216</v>
       </c>
       <c r="E107">
@@ -5825,7 +8213,7 @@
         <v>5255</v>
       </c>
       <c r="D108">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>285</v>
       </c>
       <c r="E108">
@@ -5846,7 +8234,7 @@
         <v>5348</v>
       </c>
       <c r="D109">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>68</v>
       </c>
       <c r="E109">
@@ -5867,7 +8255,7 @@
         <v>5385</v>
       </c>
       <c r="D110">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>225</v>
       </c>
       <c r="E110">
@@ -5888,7 +8276,7 @@
         <v>5435</v>
       </c>
       <c r="D111">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>35</v>
       </c>
       <c r="E111">
@@ -5909,7 +8297,7 @@
         <v>5474</v>
       </c>
       <c r="D112">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>54</v>
       </c>
       <c r="E112">
@@ -5930,7 +8318,7 @@
         <v>5506</v>
       </c>
       <c r="D113">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>36</v>
       </c>
       <c r="E113">
@@ -5951,7 +8339,7 @@
         <v>5522</v>
       </c>
       <c r="D114">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>22</v>
       </c>
       <c r="E114">
@@ -5972,7 +8360,7 @@
         <v>5545</v>
       </c>
       <c r="D115">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3295</v>
       </c>
       <c r="E115">
@@ -5993,7 +8381,7 @@
         <v>5581</v>
       </c>
       <c r="D116">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>31</v>
       </c>
       <c r="E116">
@@ -6014,7 +8402,7 @@
         <v>5701</v>
       </c>
       <c r="D117">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>81</v>
       </c>
       <c r="E117">
@@ -6035,7 +8423,7 @@
         <v>5724</v>
       </c>
       <c r="D118">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>154</v>
       </c>
       <c r="E118">
@@ -6056,7 +8444,7 @@
         <v>5766</v>
       </c>
       <c r="D119">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>46</v>
       </c>
       <c r="E119">
@@ -6077,7 +8465,7 @@
         <v>5820</v>
       </c>
       <c r="D120">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>70</v>
       </c>
       <c r="E120">
@@ -6098,7 +8486,7 @@
         <v>5864</v>
       </c>
       <c r="D121">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>74</v>
       </c>
       <c r="E121">
@@ -6119,7 +8507,7 @@
         <v>5986</v>
       </c>
       <c r="D122">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>26</v>
       </c>
       <c r="E122">

</xml_diff>